<commit_message>
allow temporarily skip some URLs
</commit_message>
<xml_diff>
--- a/scripts/python/web-monitor/monitored-urls.xlsx
+++ b/scripts/python/web-monitor/monitored-urls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\linux\scripts\python\web-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4BBDBE-916C-41E6-931F-A3FD64882F9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E28D093-36ED-4605-9DED-2B3C5684C0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18465" windowHeight="10996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Others" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>URL</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>https://www.yahoo.com/</t>
+  </si>
+  <si>
+    <t>Ignore Until</t>
+  </si>
+  <si>
+    <t>https://www.att.com</t>
+  </si>
+  <si>
+    <t>2022-05-20 23:00</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -118,6 +127,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -399,64 +410,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C389BE-3500-43A4-B395-3DEB7867D763}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="55.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
@@ -496,77 +519,82 @@
   <autoFilter ref="A1" xr:uid="{01000BF8-A878-4B65-9D09-44732CBBCBDC}"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E0908410-F68F-4963-ABC4-75AB45A47443}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{72BD674F-FBEE-40F2-B31D-DF1D7A332171}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2265544A-EDDB-4859-AA7E-14DFED1AA590}">
-  <dimension ref="A1:A324"/>
+  <dimension ref="A1:B324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="92.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
@@ -1500,5 +1528,6 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5DF4F83B-4283-4A13-8DE5-5C9D08D88906}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove httpx (no difference from requests) + retry
</commit_message>
<xml_diff>
--- a/scripts/python/web-monitor/monitored-urls.xlsx
+++ b/scripts/python/web-monitor/monitored-urls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\linux\scripts\python\web-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E28D093-36ED-4605-9DED-2B3C5684C0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931D3BEE-B798-4D74-80B6-AE70E2ECB2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Others" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>URL</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>2022-05-20 23:00</t>
+  </si>
+  <si>
+    <t>https://www.att145533.com</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -444,7 +447,9 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
@@ -520,9 +525,10 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E0908410-F68F-4963-ABC4-75AB45A47443}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{72BD674F-FBEE-40F2-B31D-DF1D7A332171}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{31765C15-CA73-4DB3-B27D-ECAC4DFE02B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
enable multi-threading for web-monitor
</commit_message>
<xml_diff>
--- a/scripts/python/web-monitor/monitored-urls.xlsx
+++ b/scripts/python/web-monitor/monitored-urls.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\linux\scripts\python\web-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931D3BEE-B798-4D74-80B6-AE70E2ECB2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D4BF27-455D-4A14-9F58-22C00A0FF0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Others" sheetId="3" r:id="rId1"/>
-    <sheet name="Internal" sheetId="4" r:id="rId2"/>
+    <sheet name="Thread1" sheetId="6" r:id="rId1"/>
+    <sheet name="Others" sheetId="3" r:id="rId2"/>
+    <sheet name="Internal" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Internal!$A$1:$A$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Others!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Internal!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Others!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Thread1!$A$1:$A$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>URL</t>
   </si>
@@ -63,6 +65,12 @@
   </si>
   <si>
     <t>https://www.att145533.com</t>
+  </si>
+  <si>
+    <t>https://www.msn.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
   </si>
 </sst>
 </file>
@@ -412,10 +420,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735BB7D8-524F-42D1-8B80-10DFAF88A1C2}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="55.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1" xr:uid="{01000BF8-A878-4B65-9D09-44732CBBCBDC}"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0C6F71E7-B558-4564-B3FE-3F34ECB8B52A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{502691D3-7526-4501-A6FE-573CC1A6CD9D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C389BE-3500-43A4-B395-3DEB7867D763}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -532,7 +656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2265544A-EDDB-4859-AA7E-14DFED1AA590}">
   <dimension ref="A1:B324"/>
   <sheetViews>

</xml_diff>